<commit_message>
Making changes to Lab 33
</commit_message>
<xml_diff>
--- a/33_ms_lake/ms_lake_data.xlsx
+++ b/33_ms_lake/ms_lake_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
   <si>
     <t>Variable</t>
   </si>
@@ -296,6 +296,36 @@
   </si>
   <si>
     <t>129/88</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>Chart initial</t>
+  </si>
+  <si>
+    <t>Blood test, initial</t>
+  </si>
+  <si>
+    <t>Blood chemistry, initial</t>
+  </si>
+  <si>
+    <t>Initial, diet</t>
+  </si>
+  <si>
+    <t>Intial, urine</t>
+  </si>
+  <si>
+    <t>Initial, blood chemistry</t>
+  </si>
+  <si>
+    <t>Lowering Sodium Intake</t>
+  </si>
+  <si>
+    <t>Blocking AngII, 70%</t>
+  </si>
+  <si>
+    <t>Lowering Sodium and Blocking AngII</t>
   </si>
 </sst>
 </file>
@@ -448,6 +478,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -459,9 +492,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:D55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -769,9 +799,10 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="48" thickBot="1">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="45.75" thickBot="1">
+    <row r="2" spans="1:5" ht="30.75" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -798,8 +829,11 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -813,7 +847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30.75" thickBot="1">
+    <row r="4" spans="1:5" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -827,7 +861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45.75" thickBot="1">
+    <row r="5" spans="1:5" ht="30.75" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -841,8 +875,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+    <row r="8" spans="1:5" ht="15.75" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -870,7 +904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -883,8 +917,11 @@
       <c r="D9" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
@@ -898,7 +935,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -912,8 +949,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="13" spans="1:4" ht="16.5" thickBot="1">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="13" spans="1:5" ht="16.5" thickBot="1">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -927,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
@@ -940,8 +977,11 @@
       <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -955,7 +995,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -969,7 +1009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+    <row r="17" spans="1:5" ht="15.75" thickBot="1">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -983,7 +1023,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1">
+    <row r="18" spans="1:5" ht="15.75" thickBot="1">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
@@ -997,7 +1037,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1">
+    <row r="19" spans="1:5" ht="15.75" thickBot="1">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -1011,7 +1051,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1">
+    <row r="20" spans="1:5" ht="15.75" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>30</v>
       </c>
@@ -1025,8 +1065,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="22" spans="1:4" ht="16.5" thickBot="1">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="22" spans="1:5" ht="16.5" thickBot="1">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30.75" thickBot="1">
+    <row r="23" spans="1:5" ht="30.75" thickBot="1">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -1053,8 +1093,11 @@
       <c r="D23" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30.75" thickBot="1">
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30.75" thickBot="1">
       <c r="A24" s="3" t="s">
         <v>33</v>
       </c>
@@ -1068,50 +1111,50 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="8" t="s">
+    <row r="25" spans="1:5">
+      <c r="A25" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="11">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="11">
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75">
-      <c r="A28" s="12" t="s">
+    <row r="28" spans="1:5" ht="15.75">
+      <c r="A28" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75">
-      <c r="A29" s="12" t="s">
+    <row r="29" spans="1:5" ht="15.75">
+      <c r="A29" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75">
-      <c r="A30" s="12" t="s">
+    <row r="30" spans="1:5" ht="15.75">
+      <c r="A30" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15.75">
-      <c r="A32" s="12" t="s">
+    <row r="32" spans="1:5" ht="15.75">
+      <c r="A32" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="34" spans="1:4" ht="16.5" thickBot="1">
+    <row r="33" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="34" spans="1:5" ht="16.5" thickBot="1">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1">
+    <row r="35" spans="1:5" ht="15.75" thickBot="1">
       <c r="A35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1138,8 +1181,11 @@
       <c r="D35" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1">
       <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
@@ -1152,9 +1198,12 @@
       <c r="D36" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="38" spans="1:4" ht="16.5" thickBot="1">
+      <c r="E36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="38" spans="1:5" ht="16.5" thickBot="1">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -1168,7 +1217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30.75" thickBot="1">
+    <row r="39" spans="1:5" ht="30.75" thickBot="1">
       <c r="A39" s="3" t="s">
         <v>45</v>
       </c>
@@ -1181,9 +1230,12 @@
       <c r="D39" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="41" spans="1:4" ht="16.5" thickBot="1">
+      <c r="E39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="41" spans="1:5" ht="16.5" thickBot="1">
       <c r="A41" s="1" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1">
+    <row r="42" spans="1:5" ht="15.75" thickBot="1">
       <c r="A42" s="3" t="s">
         <v>47</v>
       </c>
@@ -1210,8 +1262,11 @@
       <c r="D42" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1">
+      <c r="E42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" thickBot="1">
       <c r="A43" s="3" t="s">
         <v>48</v>
       </c>
@@ -1225,7 +1280,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1">
+    <row r="44" spans="1:5" ht="15.75" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>50</v>
       </c>
@@ -1239,7 +1294,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15.75" thickBot="1">
+    <row r="45" spans="1:5" ht="15.75" thickBot="1">
       <c r="A45" s="3" t="s">
         <v>51</v>
       </c>
@@ -1253,7 +1308,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1">
+    <row r="46" spans="1:5" ht="15.75" thickBot="1">
       <c r="A46" s="3" t="s">
         <v>53</v>
       </c>
@@ -1267,8 +1322,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="48" spans="1:4" ht="16.5" thickBot="1">
+    <row r="47" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="48" spans="1:5" ht="16.5" thickBot="1">
       <c r="A48" s="1" t="s">
         <v>0</v>
       </c>
@@ -1282,7 +1337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30.75" thickBot="1">
+    <row r="49" spans="1:5" ht="30.75" thickBot="1">
       <c r="A49" s="3" t="s">
         <v>4</v>
       </c>
@@ -1295,9 +1350,12 @@
       <c r="D49" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="51" spans="1:4" ht="16.5" thickBot="1">
+      <c r="E49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="51" spans="1:5" ht="16.5" thickBot="1">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30.75" thickBot="1">
+    <row r="52" spans="1:5" ht="30.75" thickBot="1">
       <c r="A52" s="3" t="s">
         <v>4</v>
       </c>
@@ -1324,9 +1382,12 @@
       <c r="D52" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1"/>
-    <row r="54" spans="1:4" ht="16.5" thickBot="1">
+      <c r="E52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" thickBot="1"/>
+    <row r="54" spans="1:5" ht="16.5" thickBot="1">
       <c r="A54" s="1" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30.75" thickBot="1">
+    <row r="55" spans="1:5" ht="30.75" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>4</v>
       </c>
@@ -1352,6 +1413,9 @@
       </c>
       <c r="D55" s="5" t="s">
         <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>